<commit_message>
Correct many names, refactor the code, delete unnecessary functions, change some variables' values
</commit_message>
<xml_diff>
--- a/templates/template.xlsx
+++ b/templates/template.xlsx
@@ -23,38 +23,35 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t xml:space="preserve">FROM</t>
   </si>
   <si>
-    <t xml:space="preserve">PrintPro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">450 Provencher Blvd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Winnipeg, MB R2J 0B9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">204-889-3030</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   sales@printprodigital.com</t>
+    <t xml:space="preserve">Your Company</t>
+  </si>
+  <si>
+    <t xml:space="preserve">777 Your St.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Winnipeg, MB R0R 0R0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">204-777-0000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     sales@yourcompany.com</t>
   </si>
   <si>
     <t xml:space="preserve">SHIP TO</t>
   </si>
   <si>
-    <t xml:space="preserve">Manitoba Motor Dealers Association</t>
+    <t xml:space="preserve">Doodoo Dynamics</t>
   </si>
   <si>
     <t xml:space="preserve">123 Anywhere Street hahaha – unit # 09099090</t>
   </si>
   <si>
-    <t xml:space="preserve">Winnipeg, MB R0R 0R0</t>
-  </si>
-  <si>
     <t xml:space="preserve">ATTN: John Doe</t>
   </si>
   <si>
@@ -64,19 +61,13 @@
     <t xml:space="preserve">JOB DETAILS</t>
   </si>
   <si>
-    <t xml:space="preserve">Order # 99999</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PO # ABC000123</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tickets - Christmas Fundraiser / Tickets - Christmas Fundraiser</t>
+    <t xml:space="preserve">Invoice # 99999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Awesome Product</t>
   </si>
   <si>
     <t xml:space="preserve">Total qty: 10000  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">#001 - 5000</t>
   </si>
   <si>
     <t xml:space="preserve">Qty in this box: 5000  </t>
@@ -89,7 +80,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -160,14 +151,6 @@
     </font>
     <font>
       <sz val="20"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="13"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -343,8 +326,8 @@
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -367,20 +350,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>275760</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>255600</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>41760</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>2030760</xdr:colOff>
+      <xdr:colOff>2402640</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>83520</xdr:rowOff>
+      <xdr:rowOff>193320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="Picture 4" descr=""/>
+        <xdr:cNvPr id="0" name="Image 1" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -389,8 +372,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3372480" y="41760"/>
-          <a:ext cx="1755000" cy="581400"/>
+          <a:off x="3088440" y="0"/>
+          <a:ext cx="2410920" cy="732960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -413,7 +396,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -488,7 +471,7 @@
     <row r="7" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="2"/>
       <c r="C7" s="6" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="17"/>
@@ -497,50 +480,46 @@
       <c r="A8" s="2"/>
       <c r="B8" s="10"/>
       <c r="C8" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="26.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="19"/>
     </row>
     <row r="10" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="2"/>
-      <c r="C10" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="7"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="0"/>
       <c r="E10" s="20"/>
     </row>
     <row r="11" customFormat="false" ht="49.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="2"/>
       <c r="C11" s="21" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E11" s="22"/>
     </row>
     <row r="12" customFormat="false" ht="22.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="2"/>
       <c r="B12" s="10"/>
-      <c r="C12" s="11" t="s">
-        <v>17</v>
-      </c>
+      <c r="C12" s="11"/>
       <c r="D12" s="18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E12" s="18"/>
     </row>
@@ -553,7 +532,7 @@
     <mergeCell ref="D12:E12"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E4" r:id="rId1" display="   sales@printprodigital.com"/>
+    <hyperlink ref="E4" r:id="rId1" display="     sales@yourcompany.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="true"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>